<commit_message>
add oled and new picture
</commit_message>
<xml_diff>
--- a/Document/报告（源文件）/设计数据/ASH067476_智信同德_物料清单.xlsx
+++ b/Document/报告（源文件）/设计数据/ASH067476_智信同德_物料清单.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\ZhixinTongde_WJ100\Document\报告（源文件）\设计数据\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\ZhixinTongde_WJ100\Document\报告（源文件）\设计数据\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EDB2D5-4017-4036-877A-924F66D1F841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AF12C6-31F1-4950-9F31-CFF684015A67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,12 +88,18 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>0.96寸Oled显示屏</t>
+  </si>
+  <si>
+    <t>龙邱科技</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +134,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +155,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -166,11 +185,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -184,6 +231,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,11 +518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="343" zoomScaleNormal="343" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -536,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -547,6 +600,20 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>